<commit_message>
seed data by mehar
</commit_message>
<xml_diff>
--- a/Group4 no preq.xlsx
+++ b/Group4 no preq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree Requirement" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="92">
   <si>
     <t>DegreeRequirementID</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>533976`</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -318,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +352,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -362,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -388,6 +397,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -670,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,9 +693,10 @@
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -693,8 +706,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -704,8 +720,12 @@
       <c r="C2" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>"new Degree{"&amp; $A$1 &amp;" =  "&amp; A2 &amp;"," &amp;$B$1 &amp; " =  '" &amp; B2 &amp; " ' ," &amp; $C$1 &amp; " = ' " &amp; $C2 &amp; "' },"</f>
+        <v>new Degree{DegreeID(PK) =  1,DegreeAbbrev =  ' ACS + 2 ' ,NumberOfTerms = ' 5' },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -715,8 +735,12 @@
       <c r="C3" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D5" si="0">"new Degree{"&amp; $A$1 &amp;" =  "&amp; A3 &amp;"," &amp;$B$1 &amp; " =  '" &amp; B3 &amp; " ' ," &amp; $C$1 &amp; " = ' " &amp; $C3 &amp; "' },"</f>
+        <v>new Degree{DegreeID(PK) =  2,DegreeAbbrev =  'ACS+DB ' ,NumberOfTerms = ' 5' },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -726,8 +750,12 @@
       <c r="C4" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Degree{DegreeID(PK) =  3,DegreeAbbrev =  'ACS+NF ' ,NumberOfTerms = ' 5' },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -736,6 +764,10 @@
       </c>
       <c r="C5" s="1">
         <v>5</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Degree{DegreeID(PK) =  4,DegreeAbbrev =  'ACS ' ,NumberOfTerms = ' 5' },</v>
       </c>
     </row>
   </sheetData>
@@ -1527,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,9 +1572,10 @@
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -1558,8 +1591,11 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1234</v>
       </c>
@@ -1575,8 +1611,12 @@
       <c r="E2" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>"new DegreePlan {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", " &amp;$C$1 &amp;"='" &amp;C2 &amp; "', "&amp;$D$1 &amp;"='" &amp;D2 &amp; "', "&amp;$E$1 &amp;"=" &amp;E2 &amp; "}"</f>
+        <v>new DegreePlan {DegreePlanID(pk)=1234, StudentID(fk)=533904, DegereePlanAbbrev='Slow and easy', DegreePlanName='Without Summer', DegreeRequirementID=4}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1235</v>
       </c>
@@ -1592,8 +1632,12 @@
       <c r="E3" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F9" si="0">"new DegreePlan {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", " &amp;$C$1 &amp;"='" &amp;C3 &amp; "', "&amp;$D$1 &amp;"='" &amp;D3 &amp; "', "&amp;$E$1 &amp;"=" &amp;E3 &amp; "}"</f>
+        <v>new DegreePlan {DegreePlanID(pk)=1235, StudentID(fk)=533904, DegereePlanAbbrev='Super Fast', DegreePlanName='With Summer', DegreeRequirementID=4}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1236</v>
       </c>
@@ -1609,8 +1653,12 @@
       <c r="E4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID(pk)=1236, StudentID(fk)=533489, DegereePlanAbbrev='Super Fast', DegreePlanName='With Summer', DegreeRequirementID=4}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1237</v>
       </c>
@@ -1626,8 +1674,12 @@
       <c r="E5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID(pk)=1237, StudentID(fk)=533489, DegereePlanAbbrev='Slow and easy', DegreePlanName='Without Summer', DegreeRequirementID=4}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1238</v>
       </c>
@@ -1643,8 +1695,12 @@
       <c r="E6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID(pk)=1238, StudentID(fk)=533976, DegereePlanAbbrev='Slow and easy', DegreePlanName='Without Summer', DegreeRequirementID=4}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1239</v>
       </c>
@@ -1660,8 +1716,12 @@
       <c r="E7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID(pk)=1239, StudentID(fk)=533976, DegereePlanAbbrev='Super Fast', DegreePlanName='With Summer', DegreeRequirementID=4}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1240</v>
       </c>
@@ -1677,8 +1737,12 @@
       <c r="E8" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID(pk)=1240, StudentID(fk)=533714, DegereePlanAbbrev='Super Fast', DegreePlanName='With Summer', DegreeRequirementID=4}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1241</v>
       </c>
@@ -1694,38 +1758,42 @@
       <c r="E9" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID(pk)=1241, StudentID(fk)=533714, DegereePlanAbbrev='Slow and easy', DegreePlanName='Without Summer', DegreeRequirementID=4}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1807,19 +1875,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="93.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -1835,8 +1905,11 @@
       <c r="E1" s="1">
         <v>919</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>533904</v>
       </c>
@@ -1852,8 +1925,12 @@
       <c r="E2" s="1">
         <v>91957050</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>"new Student {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"='" &amp;B2 &amp; "', "&amp;$C$1 &amp;"='" &amp;C2 &amp; "', "&amp;$D$1 &amp;"=" &amp;D2 &amp;"}"</f>
+        <v>new Student {StudentID(pk)=533904, Family='Peddi', Given='Taraka', Snumber=S533904}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
@@ -1869,8 +1946,12 @@
       <c r="E3" s="1">
         <v>919571539</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F5" si="0">"new Student {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"='" &amp;B3 &amp; "', "&amp;$C$1 &amp;"='" &amp;C3 &amp; "', "&amp;$D$1 &amp;"=" &amp;D3 &amp;"}"</f>
+        <v>new Student {StudentID(pk)=533976`, Family='Meenavilli', Given='Mehar Choudhary', Snumber=S533976}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>533489</v>
       </c>
@@ -1886,8 +1967,12 @@
       <c r="E4" s="1">
         <v>919568241</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student {StudentID(pk)=533489, Family='Dasari', Given='Venkat', Snumber=S533489}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>533714</v>
       </c>
@@ -1902,6 +1987,10 @@
       </c>
       <c r="E5" s="1">
         <v>919568635</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student {StudentID(pk)=533714, Family='Valluru', Given='Aakash', Snumber=S533714}</v>
       </c>
     </row>
   </sheetData>
@@ -1913,9 +2002,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="82.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1933,7 +2027,9 @@
       <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -1951,7 +2047,10 @@
       <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", "&amp;$C$1 &amp;"=" &amp;C2 &amp; ", "&amp;$D$1 &amp;"=" &amp;D2 &amp; ", "&amp;$E$1 &amp;"='" &amp;E2 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=1, DegreePlanID(fk)=1235, Term=1, CreditID(fk)=542, Status='C'}</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1969,7 +2068,10 @@
       <c r="E3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", "&amp;$C$1 &amp;"=" &amp;C3 &amp; ", "&amp;$D$1 &amp;"=" &amp;D3 &amp; ", "&amp;$E$1 &amp;"='" &amp;E3 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=2, DegreePlanID(fk)=1235, Term=1, CreditID(fk)=563, Status='C'}</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1987,7 +2089,10 @@
       <c r="E4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="str">
+        <f t="shared" ref="F4:F12" si="0">"new Slot {" &amp;$A$1 &amp;"=" &amp;A4 &amp; ", " &amp;$B$1 &amp;"=" &amp;B4 &amp; ", "&amp;$C$1 &amp;"=" &amp;C4 &amp; ", "&amp;$D$1 &amp;"=" &amp;D4 &amp; ", "&amp;$E$1 &amp;"='" &amp;E4 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=3, DegreePlanID(fk)=1235, Term=1, CreditID(fk)=560, Status='C'}</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -2005,7 +2110,10 @@
       <c r="E5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID(pk)=4, DegreePlanID(fk)=1235, Term=2, CreditID(fk)=644, Status='A'}</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -2023,7 +2131,10 @@
       <c r="E6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID(pk)=5, DegreePlanID(fk)=1235, Term=2, CreditID(fk)=664, Status='A'}</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -2041,7 +2152,10 @@
       <c r="E7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID(pk)=6, DegreePlanID(fk)=1235, Term=2, CreditID(fk)=6, Status='A'}</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -2059,7 +2173,10 @@
       <c r="E8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID(pk)=7, DegreePlanID(fk)=1235, Term=3, CreditID(fk)=618, Status='P'}</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -2077,7 +2194,10 @@
       <c r="E9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID(pk)=8, DegreePlanID(fk)=1235, Term=3, CreditID(fk)=691, Status='P'}</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2095,7 +2215,10 @@
       <c r="E10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID(pk)=9, DegreePlanID(fk)=1235, Term=4, CreditID(fk)=692, Status='P'}</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2113,7 +2236,10 @@
       <c r="E11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID(pk)=10, DegreePlanID(fk)=1235, Term=4, CreditID(fk)=2, Status='P'}</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -2131,7 +2257,10 @@
       <c r="E12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID(pk)=11, DegreePlanID(fk)=1235, Term=4, CreditID(fk)=555, Status='P'}</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -2149,7 +2278,10 @@
       <c r="E13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A13 &amp; ", " &amp;$B$1 &amp;"=" &amp;B13 &amp; ", "&amp;$C$1 &amp;"=" &amp;C13 &amp; ", "&amp;$D$1 &amp;"=" &amp;D13 &amp; ", "&amp;$E$1 &amp;"='" &amp;E13 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=12, DegreePlanID(fk)=1236, Term=1, CreditID(fk)=542, Status='A'}</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -2167,7 +2299,10 @@
       <c r="E14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A14 &amp; ", " &amp;$B$1 &amp;"=" &amp;B14 &amp; ", "&amp;$C$1 &amp;"=" &amp;C14 &amp; ", "&amp;$D$1 &amp;"=" &amp;D14 &amp; ", "&amp;$E$1 &amp;"='" &amp;E14 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=13, DegreePlanID(fk)=1236, Term=1, CreditID(fk)=563, Status='A'}</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -2185,7 +2320,10 @@
       <c r="E15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="str">
+        <f t="shared" ref="F15:F23" si="1">"new Slot {" &amp;$A$1 &amp;"=" &amp;A15 &amp; ", " &amp;$B$1 &amp;"=" &amp;B15 &amp; ", "&amp;$C$1 &amp;"=" &amp;C15 &amp; ", "&amp;$D$1 &amp;"=" &amp;D15 &amp; ", "&amp;$E$1 &amp;"='" &amp;E15 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=14, DegreePlanID(fk)=1236, Term=1, CreditID(fk)=560, Status='A'}</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -2203,7 +2341,10 @@
       <c r="E16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new Slot {SlotID(pk)=15, DegreePlanID(fk)=1236, Term=2, CreditID(fk)=618, Status='P'}</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -2221,7 +2362,10 @@
       <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new Slot {SlotID(pk)=16, DegreePlanID(fk)=1236, Term=2, CreditID(fk)=1, Status='P'}</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -2239,7 +2383,10 @@
       <c r="E18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new Slot {SlotID(pk)=17, DegreePlanID(fk)=1236, Term=3, CreditID(fk)=691, Status='P'}</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -2257,7 +2404,10 @@
       <c r="E19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new Slot {SlotID(pk)=18, DegreePlanID(fk)=1236, Term=3, CreditID(fk)=6, Status='P'}</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -2275,7 +2425,10 @@
       <c r="E20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new Slot {SlotID(pk)=19, DegreePlanID(fk)=1236, Term=3, CreditID(fk)=664, Status='P'}</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -2293,7 +2446,10 @@
       <c r="E21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new Slot {SlotID(pk)=20, DegreePlanID(fk)=1236, Term=4, CreditID(fk)=692, Status='P'}</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -2311,7 +2467,10 @@
       <c r="E22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new Slot {SlotID(pk)=21, DegreePlanID(fk)=1236, Term=4, CreditID(fk)=555, Status='P'}</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -2329,7 +2488,10 @@
       <c r="E23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new Slot {SlotID(pk)=22, DegreePlanID(fk)=1236, Term=4, CreditID(fk)=2, Status='P'}</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -2347,7 +2509,10 @@
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A24 &amp; ", " &amp;$B$1 &amp;"=" &amp;B24 &amp; ", "&amp;$C$1 &amp;"=" &amp;C24 &amp; ", "&amp;$D$1 &amp;"=" &amp;D24 &amp; ", "&amp;$E$1 &amp;"='" &amp;E24 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=23, DegreePlanID(fk)=1239, Term=1, CreditID(fk)=542, Status='C'}</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -2365,7 +2530,10 @@
       <c r="E25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A25 &amp; ", " &amp;$B$1 &amp;"=" &amp;B25 &amp; ", "&amp;$C$1 &amp;"=" &amp;C25 &amp; ", "&amp;$D$1 &amp;"=" &amp;D25 &amp; ", "&amp;$E$1 &amp;"='" &amp;E25 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=24, DegreePlanID(fk)=1239, Term=1, CreditID(fk)=563, Status='C'}</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -2383,7 +2551,10 @@
       <c r="E26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="str">
+        <f t="shared" ref="F26:F34" si="2">"new Slot {" &amp;$A$1 &amp;"=" &amp;A26 &amp; ", " &amp;$B$1 &amp;"=" &amp;B26 &amp; ", "&amp;$C$1 &amp;"=" &amp;C26 &amp; ", "&amp;$D$1 &amp;"=" &amp;D26 &amp; ", "&amp;$E$1 &amp;"='" &amp;E26 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=25, DegreePlanID(fk)=1239, Term=1, CreditID(fk)=560, Status='C'}</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -2401,7 +2572,10 @@
       <c r="E27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>new Slot {SlotID(pk)=26, DegreePlanID(fk)=1239, Term=2, CreditID(fk)=644, Status='A'}</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -2419,7 +2593,10 @@
       <c r="E28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>new Slot {SlotID(pk)=27, DegreePlanID(fk)=1239, Term=2, CreditID(fk)=664, Status='A'}</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -2437,7 +2614,10 @@
       <c r="E29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>new Slot {SlotID(pk)=28, DegreePlanID(fk)=1239, Term=2, CreditID(fk)=6, Status='A'}</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -2455,7 +2635,10 @@
       <c r="E30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>new Slot {SlotID(pk)=29, DegreePlanID(fk)=1239, Term=3, CreditID(fk)=618, Status='P'}</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -2473,6 +2656,10 @@
       <c r="E31" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="F31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>new Slot {SlotID(pk)=30, DegreePlanID(fk)=1239, Term=3, CreditID(fk)=691, Status='P'}</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -2490,8 +2677,12 @@
       <c r="E32" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>new Slot {SlotID(pk)=31, DegreePlanID(fk)=1239, Term=4, CreditID(fk)=692, Status='P'}</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2507,8 +2698,12 @@
       <c r="E33" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>new Slot {SlotID(pk)=32, DegreePlanID(fk)=1239, Term=4, CreditID(fk)=2, Status='P'}</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2524,8 +2719,12 @@
       <c r="E34" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>new Slot {SlotID(pk)=33, DegreePlanID(fk)=1239, Term=4, CreditID(fk)=555, Status='P'}</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2541,8 +2740,12 @@
       <c r="E35" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A35 &amp; ", " &amp;$B$1 &amp;"=" &amp;B35 &amp; ", "&amp;$C$1 &amp;"=" &amp;C35 &amp; ", "&amp;$D$1 &amp;"=" &amp;D35 &amp; ", "&amp;$E$1 &amp;"='" &amp;E35 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=34, DegreePlanID(fk)=1240, Term=1, CreditID(fk)=542, Status='A'}</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2558,8 +2761,12 @@
       <c r="E36" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A36 &amp; ", " &amp;$B$1 &amp;"=" &amp;B36 &amp; ", "&amp;$C$1 &amp;"=" &amp;C36 &amp; ", "&amp;$D$1 &amp;"=" &amp;D36 &amp; ", "&amp;$E$1 &amp;"='" &amp;E36 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=35, DegreePlanID(fk)=1240, Term=1, CreditID(fk)=563, Status='A'}</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2575,8 +2782,12 @@
       <c r="E37" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="str">
+        <f t="shared" ref="F37:F45" si="3">"new Slot {" &amp;$A$1 &amp;"=" &amp;A37 &amp; ", " &amp;$B$1 &amp;"=" &amp;B37 &amp; ", "&amp;$C$1 &amp;"=" &amp;C37 &amp; ", "&amp;$D$1 &amp;"=" &amp;D37 &amp; ", "&amp;$E$1 &amp;"='" &amp;E37 &amp;"'}"</f>
+        <v>new Slot {SlotID(pk)=36, DegreePlanID(fk)=1240, Term=1, CreditID(fk)=560, Status='A'}</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2592,8 +2803,12 @@
       <c r="E38" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>new Slot {SlotID(pk)=37, DegreePlanID(fk)=1240, Term=2, CreditID(fk)=618, Status='P'}</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2609,8 +2824,12 @@
       <c r="E39" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>new Slot {SlotID(pk)=38, DegreePlanID(fk)=1240, Term=2, CreditID(fk)=1, Status='P'}</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2626,8 +2845,12 @@
       <c r="E40" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>new Slot {SlotID(pk)=39, DegreePlanID(fk)=1240, Term=3, CreditID(fk)=691, Status='P'}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2643,8 +2866,12 @@
       <c r="E41" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>new Slot {SlotID(pk)=40, DegreePlanID(fk)=1240, Term=3, CreditID(fk)=6, Status='P'}</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2660,8 +2887,12 @@
       <c r="E42" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>new Slot {SlotID(pk)=41, DegreePlanID(fk)=1240, Term=3, CreditID(fk)=664, Status='P'}</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2677,8 +2908,12 @@
       <c r="E43" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>new Slot {SlotID(pk)=42, DegreePlanID(fk)=1240, Term=4, CreditID(fk)=692, Status='P'}</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2694,8 +2929,12 @@
       <c r="E44" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>new Slot {SlotID(pk)=43, DegreePlanID(fk)=1240, Term=4, CreditID(fk)=555, Status='P'}</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2711,22 +2950,26 @@
       <c r="E45" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>new Slot {SlotID(pk)=44, DegreePlanID(fk)=1240, Term=4, CreditID(fk)=2, Status='P'}</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -2940,10 +3183,10 @@
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="116.5703125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -2959,7 +3202,9 @@
       <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2978,7 +3223,10 @@
       <c r="E2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="11" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", "&amp;$C$1 &amp;"=" &amp;C2 &amp; ", "&amp;$D$1 &amp;"='" &amp;D2 &amp; "', "&amp;$E$1 &amp;"='" &amp;E2 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=1,  StudentID(fk)=533904, Term(fk)=1, TermAbbr='F18', TermName='Fall2018'}</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2997,7 +3245,10 @@
       <c r="E3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="11" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", "&amp;$C$1 &amp;"=" &amp;C3 &amp; ", "&amp;$D$1 &amp;"='" &amp;D3 &amp; "', "&amp;$E$1 &amp;"='" &amp;E3 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=2,  StudentID(fk)=533904, Term(fk)=2, TermAbbr='S19', TermName='Spring2019'}</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3016,7 +3267,10 @@
       <c r="E4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="11" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A4 &amp; ", " &amp;$B$1 &amp;"=" &amp;B4 &amp; ", "&amp;$C$1 &amp;"=" &amp;C4 &amp; ", "&amp;$D$1 &amp;"='" &amp;D4 &amp; "', "&amp;$E$1 &amp;"='" &amp;E4 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=3,  StudentID(fk)=533904, Term(fk)=3, TermAbbr='Su19', TermName='Summer2019'}</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,7 +3289,10 @@
       <c r="E5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="11" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A5 &amp; ", " &amp;$B$1 &amp;"=" &amp;B5 &amp; ", "&amp;$C$1 &amp;"=" &amp;C5 &amp; ", "&amp;$D$1 &amp;"='" &amp;D5 &amp; "', "&amp;$E$1 &amp;"='" &amp;E5 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=4,  StudentID(fk)=533904, Term(fk)=4, TermAbbr='F19', TermName='Fall2019'}</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3054,7 +3311,10 @@
       <c r="E6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A6 &amp; ", " &amp;$B$1 &amp;"=" &amp;B6 &amp; ", "&amp;$C$1 &amp;"=" &amp;C6 &amp; ", "&amp;$D$1 &amp;"='" &amp;D6 &amp; "', "&amp;$E$1 &amp;"='" &amp;E6 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=5,  StudentID(fk)=533489, Term(fk)=3, TermAbbr='S18', TermName='Spring2018'}</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3073,7 +3333,10 @@
       <c r="E7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="6" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A7 &amp; ", " &amp;$B$1 &amp;"=" &amp;B7 &amp; ", "&amp;$C$1 &amp;"=" &amp;C7 &amp; ", "&amp;$D$1 &amp;"='" &amp;D7 &amp; "', "&amp;$E$1 &amp;"='" &amp;E7 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=6,  StudentID(fk)=533489, Term(fk)=4, TermAbbr='Su18', TermName='Summer2018'}</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3092,7 +3355,10 @@
       <c r="E8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="6" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A8 &amp; ", " &amp;$B$1 &amp;"=" &amp;B8 &amp; ", "&amp;$C$1 &amp;"=" &amp;C8 &amp; ", "&amp;$D$1 &amp;"='" &amp;D8 &amp; "', "&amp;$E$1 &amp;"='" &amp;E8 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=7,  StudentID(fk)=533489, Term(fk)=5, TermAbbr='F18', TermName='Fall2018'}</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3111,7 +3377,10 @@
       <c r="E9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="6" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A9 &amp; ", " &amp;$B$1 &amp;"=" &amp;B9 &amp; ", "&amp;$C$1 &amp;"=" &amp;C9 &amp; ", "&amp;$D$1 &amp;"='" &amp;D9 &amp; "', "&amp;$E$1 &amp;"='" &amp;E9 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=8,  StudentID(fk)=533489, Term(fk)=6, TermAbbr='S19', TermName='Spring2019'}</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3130,7 +3399,10 @@
       <c r="E10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="4" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A10 &amp; ", " &amp;$B$1 &amp;"=" &amp;B10 &amp; ", "&amp;$C$1 &amp;"=" &amp;C10 &amp; ", "&amp;$D$1 &amp;"='" &amp;D10 &amp; "', "&amp;$E$1 &amp;"='" &amp;E10 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=9,  StudentID(fk)=533976, Term(fk)=1, TermAbbr='F19', TermName='Fall2019'}</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3149,7 +3421,10 @@
       <c r="E11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="4" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A11 &amp; ", " &amp;$B$1 &amp;"=" &amp;B11 &amp; ", "&amp;$C$1 &amp;"=" &amp;C11 &amp; ", "&amp;$D$1 &amp;"='" &amp;D11 &amp; "', "&amp;$E$1 &amp;"='" &amp;E11 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=10,  StudentID(fk)=533976, Term(fk)=2, TermAbbr='S20', TermName='Spring2020'}</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3168,7 +3443,10 @@
       <c r="E12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="4" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A12 &amp; ", " &amp;$B$1 &amp;"=" &amp;B12 &amp; ", "&amp;$C$1 &amp;"=" &amp;C12 &amp; ", "&amp;$D$1 &amp;"='" &amp;D12 &amp; "', "&amp;$E$1 &amp;"='" &amp;E12 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=11,  StudentID(fk)=533976, Term(fk)=3, TermAbbr='Su20', TermName='Summer2020'}</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3187,7 +3465,10 @@
       <c r="E13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="4" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A13 &amp; ", " &amp;$B$1 &amp;"=" &amp;B13 &amp; ", "&amp;$C$1 &amp;"=" &amp;C13 &amp; ", "&amp;$D$1 &amp;"='" &amp;D13 &amp; "', "&amp;$E$1 &amp;"='" &amp;E13 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=12,  StudentID(fk)=533976, Term(fk)=4, TermAbbr='F20', TermName='Fall2020'}</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3206,7 +3487,10 @@
       <c r="E14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="5" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A14 &amp; ", " &amp;$B$1 &amp;"=" &amp;B14 &amp; ", "&amp;$C$1 &amp;"=" &amp;C14 &amp; ", "&amp;$D$1 &amp;"='" &amp;D14 &amp; "', "&amp;$E$1 &amp;"='" &amp;E14 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=13,  StudentID(fk)=533714, Term(fk)=3, TermAbbr='S19', TermName='Spring2019'}</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3225,7 +3509,10 @@
       <c r="E15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="5" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A15 &amp; ", " &amp;$B$1 &amp;"=" &amp;B15 &amp; ", "&amp;$C$1 &amp;"=" &amp;C15 &amp; ", "&amp;$D$1 &amp;"='" &amp;D15 &amp; "', "&amp;$E$1 &amp;"='" &amp;E15 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=14,  StudentID(fk)=533714, Term(fk)=4, TermAbbr='Su19', TermName='Summer2019'}</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3244,7 +3531,10 @@
       <c r="E16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="5" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A16 &amp; ", " &amp;$B$1 &amp;"=" &amp;B16 &amp; ", "&amp;$C$1 &amp;"=" &amp;C16 &amp; ", "&amp;$D$1 &amp;"='" &amp;D16 &amp; "', "&amp;$E$1 &amp;"='" &amp;E16 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=15,  StudentID(fk)=533714, Term(fk)=5, TermAbbr='F19', TermName='Fall2019'}</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3263,7 +3553,10 @@
       <c r="E17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="5" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A17 &amp; ", " &amp;$B$1 &amp;"=" &amp;B17 &amp; ", "&amp;$C$1 &amp;"=" &amp;C17 &amp; ", "&amp;$D$1 &amp;"='" &amp;D17 &amp; "', "&amp;$E$1 &amp;"='" &amp;E17 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTerm(pk)=16,  StudentID(fk)=533714, Term(fk)=6, TermAbbr='S20', TermName='Spring2020'}</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>

</xml_diff>